<commit_message>
Manual testing bug report
</commit_message>
<xml_diff>
--- a/FactorialWebsiteTesting_Bugs_Report.xlsx
+++ b/FactorialWebsiteTesting_Bugs_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaki\IdeaProjects\SeleniumTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2B6F699-EEDC-474E-8E38-C332033AE4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE8A4E1-CF3F-40FE-9318-4214FC3A1733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -224,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -279,6 +278,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,7 +673,7 @@
       <c r="J2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="19" t="s">
         <v>29</v>
       </c>
       <c r="L2" s="14"/>

</xml_diff>